<commit_message>
fixed incorrect names in ad index file
</commit_message>
<xml_diff>
--- a/google-ads/data/ad-index.xlsx
+++ b/google-ads/data/ad-index.xlsx
@@ -14,6 +14,9 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="64">
   <si>
     <t>NUMBER</t>
+  </si>
+  <si>
+    <t>AD ID</t>
   </si>
   <si>
     <t>POSED ON</t>
@@ -46,13 +49,13 @@
     <t>STATUS</t>
   </si>
   <si>
-    <t>AD ID</t>
+    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22932412722_6605406465_11001532719682889676_BP_SINCERITY_ORIGINSTORY_PMG_H15_V2</t>
   </si>
   <si>
     <t>English</t>
   </si>
   <si>
-    <t>World of Tanks_ HEAT - Conquer with Heavy Armor</t>
+    <t>World of Tanks: HEAT - Conquer with Heavy Armor</t>
   </si>
   <si>
     <t>Blast your way to the top!</t>
@@ -61,7 +64,7 @@
     <t>https://www.youtube.com/watch?v=9dUUrlKGR6E</t>
   </si>
   <si>
-    <t>World of Tanks_ HEAT</t>
+    <t>World of Tanks: HEAT</t>
   </si>
   <si>
     <t>https://www.youtube.com/channel/UC_dl786zjxH3keWrcLjhI9w</t>
@@ -73,7 +76,7 @@
     <t>Unlisted</t>
   </si>
   <si>
-    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22932412722_6605406465_11001532719682889676_BP_SINCERITY_ORIGINSTORY_PMG_H15_V2</t>
+    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22932412722_6605406300_16583666955524105830_GRID_PMG_H15_V1</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=tvlF0jb-rNU</t>
@@ -82,7 +85,7 @@
     <t>https://www.youtube.com/channel/UC2PqbRh89grZhFp8SB3OVng</t>
   </si>
   <si>
-    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22932412722_6605406300_16583666955524105830_GRID_PMG_H15_V1</t>
+    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22932412722_6605355095_12096389208083083760_GLITCH_PMG_V15_V1</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=CquRoX4NezQ</t>
@@ -94,13 +97,13 @@
     <t>Short</t>
   </si>
   <si>
-    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22932412722_6605355095_12096389208083083760_GLITCH_PMG_V15_V1</t>
+    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22942333141_6605406414_6991140753670039054_GRID_PMG_H15_V1</t>
   </si>
   <si>
     <t>Polish</t>
   </si>
   <si>
-    <t>World of Tanks_ HEAT - Ostateczna rozgrywka pancerna</t>
+    <t>World of Tanks: HEAT - Ostateczna rozgrywka pancerna</t>
   </si>
   <si>
     <t>Darmowa wysokooktanowa strzelanka pancerna</t>
@@ -112,7 +115,7 @@
     <t>https://www.youtube.com/channel/UCLFps42NBZr2C2i2WijWUtQ</t>
   </si>
   <si>
-    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22942333141_6605406414_6991140753670039054_GRID_PMG_H15_V1</t>
+    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22932413451_6605355059_5019121169823901274_GLITCH_PMG_V15_V1</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=QCbeENGNbkU</t>
@@ -121,7 +124,7 @@
     <t>https://www.youtube.com/channel/UCGAnFr3hh7pxkCsRul-ir-Q</t>
   </si>
   <si>
-    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22932413451_6605355059_5019121169823901274_GLITCH_PMG_V15_V1</t>
+    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22942333141_6605355035_9935253591551028359_RIPPLE_PMG_S15_V1</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=url0MnbXpkY</t>
@@ -130,7 +133,7 @@
     <t>https://www.youtube.com/channel/UC60ZD9FwJNXuRAPmY4UOfcQ</t>
   </si>
   <si>
-    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22942333141_6605355035_9935253591551028359_RIPPLE_PMG_S15_V1</t>
+    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22942333141_6605460151_4736321072828745071_CUBE_PMG_V15_V2</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=iL2LZO6xpBY</t>
@@ -139,13 +142,13 @@
     <t>https://www.youtube.com/channel/UCRYioz-8Qi6j7s_rggkr_mg</t>
   </si>
   <si>
-    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22942333141_6605460151_4736321072828745071_CUBE_PMG_V15_V2</t>
+    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22932413427_6605406417_12060199489353242383_BP_SINCERITY_ORIGINSTORY_PMG_H15_V2</t>
   </si>
   <si>
     <t>German</t>
   </si>
   <si>
-    <t>World of Tanks_ HEAT - Ultimativer Panzer-Showdown</t>
+    <t>World of Tanks: HEAT - Ultimativer Panzer-Showdown</t>
   </si>
   <si>
     <t>Tritt dem Kampf bei – Panzer, Geschütze und Ruhm erwarten dich!</t>
@@ -157,7 +160,7 @@
     <t>https://www.youtube.com/channel/UC8f1G1FBcdAPfBL4NHCrYtw</t>
   </si>
   <si>
-    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22932413427_6605406417_12060199489353242383_BP_SINCERITY_ORIGINSTORY_PMG_H15_V2</t>
+    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22932413451_6605406444_10469635398478181590_BP_SINCERITY_ORIGINSTORY_PMG_H15_V2</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=W7FCXoGjeSs</t>
@@ -166,7 +169,7 @@
     <t>https://www.youtube.com/channel/UC2n_lqFROtMZFnqVVPsWXCw</t>
   </si>
   <si>
-    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22932413451_6605406444_10469635398478181590_BP_SINCERITY_ORIGINSTORY_PMG_H15_V2</t>
+    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22932413451_6605406468_8616460694791464218_BP_SINCERITY_ORIGINSTORY_PMG_H15_V2</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=yV_n7yrxsGc</t>
@@ -175,7 +178,7 @@
     <t>https://www.youtube.com/channel/UCGhdkrOjKfaByrGN0kKoT8Q</t>
   </si>
   <si>
-    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22932413451_6605406468_8616460694791464218_BP_SINCERITY_ORIGINSTORY_PMG_H15_V2</t>
+    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22942334305_6605460088_8504706823087928205_GRID_PMG_H15_V1</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=EkC7Vn7B2JI</t>
@@ -184,7 +187,7 @@
     <t>https://www.youtube.com/channel/UCLOaryYzT1apeGbOuJwBotg</t>
   </si>
   <si>
-    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22942334305_6605460088_8504706823087928205_GRID_PMG_H15_V1</t>
+    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22932413427_6605355041_17924682452602524236_BP_SINCERITY_ORIGINSTORY_PMG_H15_V2</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=Gh4QGl3VlrE</t>
@@ -193,16 +196,13 @@
     <t>https://www.youtube.com/channel/UCyTO51OJUCOttRrDBSQ0qSg</t>
   </si>
   <si>
-    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22932413427_6605355041_17924682452602524236_BP_SINCERITY_ORIGINSTORY_PMG_H15_V2</t>
+    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22942334305_6605355047_15551527489337974589_GRID_PMG_H15_V1</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=KeZ8WqxHgsQ</t>
   </si>
   <si>
     <t>https://www.youtube.com/channel/UCqMNNDPx9TMvvvNukY4y2gw</t>
-  </si>
-  <si>
-    <t>ADIP_UBERVERSAL_GENERAL_1238106475_22942334305_6605355047_15551527489337974589_GRID_PMG_H15_V1</t>
   </si>
 </sst>
 </file>
@@ -330,17 +330,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:L1000" displayName="Table_1" name="Table_1" id="1">
   <tableColumns count="12">
     <tableColumn name="NUMBER" id="1"/>
-    <tableColumn name="POSED ON" id="2"/>
-    <tableColumn name="LAST SHOWN" id="3"/>
-    <tableColumn name="LANGUAGE" id="4"/>
-    <tableColumn name="TITLE" id="5"/>
-    <tableColumn name="DESCRIPTION" id="6"/>
-    <tableColumn name="URL" id="7"/>
-    <tableColumn name="CHANNEL NAME" id="8"/>
-    <tableColumn name="CHANNEL URL" id="9"/>
-    <tableColumn name="TYPE" id="10"/>
-    <tableColumn name="STATUS" id="11"/>
-    <tableColumn name="AD ID" id="12"/>
+    <tableColumn name="AD ID" id="2"/>
+    <tableColumn name="POSED ON" id="3"/>
+    <tableColumn name="LAST SHOWN" id="4"/>
+    <tableColumn name="LANGUAGE" id="5"/>
+    <tableColumn name="TITLE" id="6"/>
+    <tableColumn name="DESCRIPTION" id="7"/>
+    <tableColumn name="URL" id="8"/>
+    <tableColumn name="CHANNEL NAME" id="9"/>
+    <tableColumn name="CHANNEL URL" id="10"/>
+    <tableColumn name="TYPE" id="11"/>
+    <tableColumn name="STATUS" id="12"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
@@ -551,13 +551,13 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.25"/>
-    <col customWidth="1" min="2" max="2" width="19.75"/>
-    <col customWidth="1" min="3" max="3" width="19.88"/>
-    <col customWidth="1" min="4" max="4" width="19.13"/>
-    <col customWidth="1" min="5" max="7" width="25.38"/>
-    <col customWidth="1" min="8" max="8" width="25.25"/>
-    <col customWidth="1" min="9" max="9" width="25.5"/>
-    <col customWidth="1" min="12" max="12" width="25.38"/>
+    <col customWidth="1" min="2" max="2" width="25.38"/>
+    <col customWidth="1" min="3" max="3" width="19.75"/>
+    <col customWidth="1" min="4" max="4" width="19.88"/>
+    <col customWidth="1" min="5" max="5" width="19.13"/>
+    <col customWidth="1" min="6" max="8" width="25.38"/>
+    <col customWidth="1" min="9" max="9" width="25.25"/>
+    <col customWidth="1" min="10" max="10" width="25.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -602,14 +602,14 @@
       <c r="A2" s="2">
         <v>1.0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3">
         <v>45895.0</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="3">
         <v>45921.0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
@@ -617,16 +617,16 @@
       <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="K2" s="2" t="s">
@@ -640,14 +640,14 @@
       <c r="A3" s="2">
         <v>2.0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3">
         <v>45895.0</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="3">
         <v>45912.0</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>13</v>
@@ -655,37 +655,37 @@
       <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="4" t="s">
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>18</v>
+      <c r="I3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
         <v>3.0</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="3">
         <v>45895.0</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="3">
         <v>45912.0</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -693,37 +693,37 @@
       <c r="F4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="4" t="s">
+      <c r="G4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="I4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>26</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
         <v>4.0</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3">
         <v>45895.0</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="3">
         <v>45909.0</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>29</v>
@@ -731,37 +731,37 @@
       <c r="F5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>18</v>
+      <c r="I5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2">
         <v>5.0</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="3">
         <v>45895.0</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D6" s="3">
         <v>45909.0</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>13</v>
@@ -769,37 +769,37 @@
       <c r="F6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="G6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>26</v>
+      <c r="I6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
         <v>6.0</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="3">
         <v>45895.0</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="3">
         <v>45909.0</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>29</v>
@@ -807,37 +807,37 @@
       <c r="F7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="4" t="s">
+      <c r="G7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>26</v>
+      <c r="I7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
         <v>7.0</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="3">
         <v>45895.0</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="3">
         <v>45909.0</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>29</v>
@@ -845,37 +845,37 @@
       <c r="F8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="4" t="s">
+      <c r="G8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>26</v>
+      <c r="I8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
         <v>8.0</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="3">
         <v>45895.0</v>
       </c>
-      <c r="C9" s="3">
+      <c r="D9" s="3">
         <v>45909.0</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>44</v>
@@ -883,37 +883,37 @@
       <c r="F9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>18</v>
+      <c r="I9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
         <v>9.0</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="3">
         <v>45895.0</v>
       </c>
-      <c r="C10" s="3">
+      <c r="D10" s="3">
         <v>45909.0</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>13</v>
@@ -921,37 +921,37 @@
       <c r="F10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="4" t="s">
+      <c r="G10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>18</v>
+      <c r="I10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
         <v>10.0</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="3">
         <v>45895.0</v>
       </c>
-      <c r="C11" s="3">
+      <c r="D11" s="3">
         <v>45909.0</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>13</v>
@@ -959,37 +959,37 @@
       <c r="F11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="4" t="s">
+      <c r="G11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>18</v>
+      <c r="I11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
         <v>11.0</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="3">
         <v>45895.0</v>
       </c>
-      <c r="C12" s="3">
+      <c r="D12" s="3">
         <v>45909.0</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>13</v>
@@ -997,37 +997,37 @@
       <c r="F12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="4" t="s">
+      <c r="G12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>18</v>
+      <c r="I12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
         <v>12.0</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="3">
         <v>45895.0</v>
       </c>
-      <c r="C13" s="3">
+      <c r="D13" s="3">
         <v>45909.0</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>44</v>
@@ -1035,37 +1035,37 @@
       <c r="F13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="4" t="s">
+      <c r="G13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>18</v>
+      <c r="I13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2">
         <v>13.0</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="3">
         <v>45895.0</v>
       </c>
-      <c r="C14" s="3">
+      <c r="D14" s="3">
         <v>45909.0</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>13</v>
@@ -1073,43 +1073,43 @@
       <c r="F14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="4" t="s">
+      <c r="G14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>18</v>
+      <c r="I14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2"/>
       <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
+      <c r="K15" s="2"/>
       <c r="L15" s="5"/>
     </row>
     <row r="16">
       <c r="A16" s="2"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
+      <c r="C16" s="2"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -1123,7 +1123,7 @@
     <row r="17">
       <c r="A17" s="2"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+      <c r="C17" s="2"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -1137,7 +1137,7 @@
     <row r="18">
       <c r="A18" s="2"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="C18" s="2"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -1151,7 +1151,7 @@
     <row r="19">
       <c r="A19" s="2"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+      <c r="C19" s="2"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -1165,7 +1165,7 @@
     <row r="20">
       <c r="A20" s="2"/>
       <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+      <c r="C20" s="2"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -1179,7 +1179,7 @@
     <row r="21">
       <c r="A21" s="2"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+      <c r="C21" s="2"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -1193,7 +1193,7 @@
     <row r="22">
       <c r="A22" s="2"/>
       <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="C22" s="2"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -1207,7 +1207,7 @@
     <row r="23">
       <c r="A23" s="2"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+      <c r="C23" s="2"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -1221,7 +1221,7 @@
     <row r="24">
       <c r="A24" s="2"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+      <c r="C24" s="2"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -1235,7 +1235,7 @@
     <row r="25">
       <c r="A25" s="2"/>
       <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+      <c r="C25" s="2"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -1249,7 +1249,7 @@
     <row r="26">
       <c r="A26" s="2"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+      <c r="C26" s="2"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -1263,7 +1263,7 @@
     <row r="27">
       <c r="A27" s="2"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="C27" s="2"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -1277,7 +1277,7 @@
     <row r="28">
       <c r="A28" s="2"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
+      <c r="C28" s="2"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -1291,7 +1291,7 @@
     <row r="29">
       <c r="A29" s="2"/>
       <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
+      <c r="C29" s="2"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -1305,7 +1305,7 @@
     <row r="30">
       <c r="A30" s="2"/>
       <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
+      <c r="C30" s="2"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -1319,7 +1319,7 @@
     <row r="31">
       <c r="A31" s="2"/>
       <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
+      <c r="C31" s="2"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -1331,9 +1331,9 @@
       <c r="L31" s="5"/>
     </row>
     <row r="32">
-      <c r="A32" s="5"/>
+      <c r="A32" s="2"/>
       <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
+      <c r="C32" s="2"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -1345,9 +1345,9 @@
       <c r="L32" s="5"/>
     </row>
     <row r="33">
-      <c r="A33" s="5"/>
+      <c r="A33" s="2"/>
       <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
+      <c r="C33" s="2"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -1359,9 +1359,9 @@
       <c r="L33" s="5"/>
     </row>
     <row r="34">
-      <c r="A34" s="5"/>
+      <c r="A34" s="2"/>
       <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
+      <c r="C34" s="2"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -1373,9 +1373,9 @@
       <c r="L34" s="5"/>
     </row>
     <row r="35">
-      <c r="A35" s="5"/>
+      <c r="A35" s="2"/>
       <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
+      <c r="C35" s="2"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -1387,9 +1387,9 @@
       <c r="L35" s="5"/>
     </row>
     <row r="36">
-      <c r="A36" s="5"/>
+      <c r="A36" s="2"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
+      <c r="C36" s="2"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -1401,9 +1401,9 @@
       <c r="L36" s="5"/>
     </row>
     <row r="37">
-      <c r="A37" s="5"/>
+      <c r="A37" s="2"/>
       <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
+      <c r="C37" s="2"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -1415,9 +1415,9 @@
       <c r="L37" s="5"/>
     </row>
     <row r="38">
-      <c r="A38" s="5"/>
+      <c r="A38" s="2"/>
       <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
+      <c r="C38" s="2"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -1429,9 +1429,9 @@
       <c r="L38" s="5"/>
     </row>
     <row r="39">
-      <c r="A39" s="5"/>
+      <c r="A39" s="2"/>
       <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
+      <c r="C39" s="2"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -1443,9 +1443,9 @@
       <c r="L39" s="5"/>
     </row>
     <row r="40">
-      <c r="A40" s="5"/>
+      <c r="A40" s="2"/>
       <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
+      <c r="C40" s="2"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
@@ -1457,9 +1457,9 @@
       <c r="L40" s="5"/>
     </row>
     <row r="41">
-      <c r="A41" s="5"/>
+      <c r="A41" s="2"/>
       <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
+      <c r="C41" s="2"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -1471,9 +1471,9 @@
       <c r="L41" s="5"/>
     </row>
     <row r="42">
-      <c r="A42" s="5"/>
+      <c r="A42" s="2"/>
       <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
+      <c r="C42" s="2"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
@@ -1485,9 +1485,9 @@
       <c r="L42" s="5"/>
     </row>
     <row r="43">
-      <c r="A43" s="5"/>
+      <c r="A43" s="2"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
+      <c r="C43" s="2"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
@@ -1499,9 +1499,9 @@
       <c r="L43" s="5"/>
     </row>
     <row r="44">
-      <c r="A44" s="5"/>
+      <c r="A44" s="2"/>
       <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
+      <c r="C44" s="2"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
@@ -1513,9 +1513,9 @@
       <c r="L44" s="5"/>
     </row>
     <row r="45">
-      <c r="A45" s="5"/>
+      <c r="A45" s="2"/>
       <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
+      <c r="C45" s="2"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -1527,9 +1527,9 @@
       <c r="L45" s="5"/>
     </row>
     <row r="46">
-      <c r="A46" s="5"/>
+      <c r="A46" s="2"/>
       <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
+      <c r="C46" s="2"/>
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
@@ -1541,9 +1541,9 @@
       <c r="L46" s="5"/>
     </row>
     <row r="47">
-      <c r="A47" s="5"/>
+      <c r="A47" s="2"/>
       <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
+      <c r="C47" s="2"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -1555,9 +1555,9 @@
       <c r="L47" s="5"/>
     </row>
     <row r="48">
-      <c r="A48" s="5"/>
+      <c r="A48" s="2"/>
       <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
+      <c r="C48" s="2"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -1569,9 +1569,9 @@
       <c r="L48" s="5"/>
     </row>
     <row r="49">
-      <c r="A49" s="5"/>
+      <c r="A49" s="2"/>
       <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
+      <c r="C49" s="2"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -1583,9 +1583,9 @@
       <c r="L49" s="5"/>
     </row>
     <row r="50">
-      <c r="A50" s="5"/>
+      <c r="A50" s="2"/>
       <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
+      <c r="C50" s="2"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -1597,9 +1597,9 @@
       <c r="L50" s="5"/>
     </row>
     <row r="51">
-      <c r="A51" s="5"/>
+      <c r="A51" s="2"/>
       <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
+      <c r="C51" s="2"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
@@ -14898,32 +14898,32 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G2"/>
-    <hyperlink r:id="rId2" ref="I2"/>
-    <hyperlink r:id="rId3" ref="G3"/>
-    <hyperlink r:id="rId4" ref="I3"/>
-    <hyperlink r:id="rId5" ref="G4"/>
-    <hyperlink r:id="rId6" ref="I4"/>
-    <hyperlink r:id="rId7" ref="G5"/>
-    <hyperlink r:id="rId8" ref="I5"/>
-    <hyperlink r:id="rId9" ref="G6"/>
-    <hyperlink r:id="rId10" ref="I6"/>
-    <hyperlink r:id="rId11" ref="G7"/>
-    <hyperlink r:id="rId12" ref="I7"/>
-    <hyperlink r:id="rId13" ref="G8"/>
-    <hyperlink r:id="rId14" ref="I8"/>
-    <hyperlink r:id="rId15" ref="G9"/>
-    <hyperlink r:id="rId16" ref="I9"/>
-    <hyperlink r:id="rId17" ref="G10"/>
-    <hyperlink r:id="rId18" ref="I10"/>
-    <hyperlink r:id="rId19" ref="G11"/>
-    <hyperlink r:id="rId20" ref="I11"/>
-    <hyperlink r:id="rId21" ref="G12"/>
-    <hyperlink r:id="rId22" ref="I12"/>
-    <hyperlink r:id="rId23" ref="G13"/>
-    <hyperlink r:id="rId24" ref="I13"/>
-    <hyperlink r:id="rId25" ref="G14"/>
-    <hyperlink r:id="rId26" ref="I14"/>
+    <hyperlink r:id="rId1" ref="H2"/>
+    <hyperlink r:id="rId2" ref="J2"/>
+    <hyperlink r:id="rId3" ref="H3"/>
+    <hyperlink r:id="rId4" ref="J3"/>
+    <hyperlink r:id="rId5" ref="H4"/>
+    <hyperlink r:id="rId6" ref="J4"/>
+    <hyperlink r:id="rId7" ref="H5"/>
+    <hyperlink r:id="rId8" ref="J5"/>
+    <hyperlink r:id="rId9" ref="H6"/>
+    <hyperlink r:id="rId10" ref="J6"/>
+    <hyperlink r:id="rId11" ref="H7"/>
+    <hyperlink r:id="rId12" ref="J7"/>
+    <hyperlink r:id="rId13" ref="H8"/>
+    <hyperlink r:id="rId14" ref="J8"/>
+    <hyperlink r:id="rId15" ref="H9"/>
+    <hyperlink r:id="rId16" ref="J9"/>
+    <hyperlink r:id="rId17" ref="H10"/>
+    <hyperlink r:id="rId18" ref="J10"/>
+    <hyperlink r:id="rId19" ref="H11"/>
+    <hyperlink r:id="rId20" ref="J11"/>
+    <hyperlink r:id="rId21" ref="H12"/>
+    <hyperlink r:id="rId22" ref="J12"/>
+    <hyperlink r:id="rId23" ref="H13"/>
+    <hyperlink r:id="rId24" ref="J13"/>
+    <hyperlink r:id="rId25" ref="H14"/>
+    <hyperlink r:id="rId26" ref="J14"/>
   </hyperlinks>
   <drawing r:id="rId27"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
updated ad index XSLX file with image based ad details
</commit_message>
<xml_diff>
--- a/google-ads/data/ad-index.xlsx
+++ b/google-ads/data/ad-index.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="127">
   <si>
     <t>NUMBER</t>
   </si>
@@ -203,6 +203,195 @@
   </si>
   <si>
     <t>https://www.youtube.com/channel/UCqMNNDPx9TMvvvNukY4y2gw</t>
+  </si>
+  <si>
+    <t>CR13874145813908684801_1</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Jump In — Fire Away</t>
+  </si>
+  <si>
+    <t>Join the fight — tanks, guns, and glory await!</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>CR13874145813908684801_2</t>
+  </si>
+  <si>
+    <t>CR01035223303159021569_1</t>
+  </si>
+  <si>
+    <t>Hero Tank Shooter</t>
+  </si>
+  <si>
+    <t>Conquer your foes in epic armored battles.</t>
+  </si>
+  <si>
+    <t>CR01035223303159021569_2</t>
+  </si>
+  <si>
+    <t>Ultimate Tank Showdown</t>
+  </si>
+  <si>
+    <t>CR01035223303159021569_3</t>
+  </si>
+  <si>
+    <t>CR06338211864387780609_1</t>
+  </si>
+  <si>
+    <t>CR00149140076473876481_1</t>
+  </si>
+  <si>
+    <t>CR00149140076473876481_2</t>
+  </si>
+  <si>
+    <t>CR01641947013505351681_1</t>
+  </si>
+  <si>
+    <t>Choose your Agent</t>
+  </si>
+  <si>
+    <t>CR10321645734796984321_1</t>
+  </si>
+  <si>
+    <t>Walki czołgów z bohaterami. Dołącz do walki – czołgi, działa i chwała czekają!</t>
+  </si>
+  <si>
+    <t>CR04004507230526242817_1</t>
+  </si>
+  <si>
+    <t>CR04004507230526242817_2</t>
+  </si>
+  <si>
+    <t>CR06051045815491756033_1</t>
+  </si>
+  <si>
+    <t>Hero Tank Shooter. Conquer your foes in epic armored battles.</t>
+  </si>
+  <si>
+    <t>CR06502769172647247873_1</t>
+  </si>
+  <si>
+    <t>Ultimativer Panzer-Showdown. Kostenloser, adrenalingeladener Panzer-Shooter.</t>
+  </si>
+  <si>
+    <t>CR08927368233753772033_1</t>
+  </si>
+  <si>
+    <t>War Machines Unleashed. Join the fight — tanks, guns, and glory await!</t>
+  </si>
+  <si>
+    <t>CR18028369024483590145_1</t>
+  </si>
+  <si>
+    <t>CR03511077198305951745_1</t>
+  </si>
+  <si>
+    <t>CR00498556075688067073_1</t>
+  </si>
+  <si>
+    <t>CR02253258985874391041_1</t>
+  </si>
+  <si>
+    <t>CR02253258985874391041_2</t>
+  </si>
+  <si>
+    <t>War Machines Unleashed</t>
+  </si>
+  <si>
+    <t>CR02253258985874391041_3</t>
+  </si>
+  <si>
+    <t>CR04941413183182077953_1</t>
+  </si>
+  <si>
+    <t>CR04941413183182077953_2</t>
+  </si>
+  <si>
+    <t>CR04941413183182077953_3</t>
+  </si>
+  <si>
+    <t>Hero-Panzer-Shooter</t>
+  </si>
+  <si>
+    <t>Kostenloser, Adrenalingeladener Panzer-Shooter.</t>
+  </si>
+  <si>
+    <t>CR06241912237980647425_1</t>
+  </si>
+  <si>
+    <t>CR17647502594668494849_1</t>
+  </si>
+  <si>
+    <t>Ultimativer Panzer-Showdown</t>
+  </si>
+  <si>
+    <t>CR02499003133217210369_1</t>
+  </si>
+  <si>
+    <t>CR02499003133217210369_2</t>
+  </si>
+  <si>
+    <t>CR12196269079689953281_1</t>
+  </si>
+  <si>
+    <t>CR08907972848639803393_1</t>
+  </si>
+  <si>
+    <t>Free-to-play, high-octane tank shooter.</t>
+  </si>
+  <si>
+    <t>CR11765903735904010241_1</t>
+  </si>
+  <si>
+    <t>Explosive Tank Action</t>
+  </si>
+  <si>
+    <t>CR11765903735904010241_2</t>
+  </si>
+  <si>
+    <t>CR13217183218266013697_1</t>
+  </si>
+  <si>
+    <t>CR04869239040911605761_1</t>
+  </si>
+  <si>
+    <t>CR04869239040911605761_2</t>
+  </si>
+  <si>
+    <t>CR03571770240159186945_1</t>
+  </si>
+  <si>
+    <t>CR03571770240159186945_2</t>
+  </si>
+  <si>
+    <t>CR03571770240159186945_3</t>
+  </si>
+  <si>
+    <t>CR12165961041670307841_1</t>
+  </si>
+  <si>
+    <t>CR06453012972955500545_1</t>
+  </si>
+  <si>
+    <t>CR06453012972955500545_2</t>
+  </si>
+  <si>
+    <t>CR06453012972955500545_3</t>
+  </si>
+  <si>
+    <t>CR00468740618877665281_1</t>
+  </si>
+  <si>
+    <t>Conquer with Heavy Armor</t>
   </si>
 </sst>
 </file>
@@ -1093,858 +1282,1890 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="5"/>
+      <c r="A15" s="2">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="3">
+        <v>45921.0</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="2"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="A16" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="3">
+        <v>45921.0</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="2"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="A17" s="2">
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="3">
+        <v>45921.0</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="2"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
+      <c r="A18" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="3">
+        <v>45921.0</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="2"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
+      <c r="A19" s="2">
+        <v>18.0</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="3">
+        <v>45921.0</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="2"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
+      <c r="A20" s="2">
+        <v>19.0</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="3">
+        <v>45912.0</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="2"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
+      <c r="A21" s="2">
+        <v>20.0</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="3">
+        <v>45912.0</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" s="2"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
+      <c r="A22" s="2">
+        <v>21.0</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="3">
+        <v>45912.0</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="2"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
+      <c r="A23" s="2">
+        <v>22.0</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="2"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
+      <c r="A24" s="2">
+        <v>23.0</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
+      <c r="A25" s="2">
+        <v>24.0</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="2"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
+      <c r="A26" s="2">
+        <v>25.0</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="2"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
+      <c r="A27" s="2">
+        <v>26.0</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="2"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
+      <c r="A28" s="2">
+        <v>27.0</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="2"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
+      <c r="A29" s="2">
+        <v>28.0</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="2"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
+      <c r="A30" s="2">
+        <v>29.0</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="2"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
+      <c r="A31" s="2">
+        <v>30.0</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="2"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
+      <c r="A32" s="2">
+        <v>31.0</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="2"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
+      <c r="A33" s="2">
+        <v>32.0</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="2"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
+      <c r="A34" s="2">
+        <v>33.0</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="2"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
+      <c r="A35" s="2">
+        <v>34.0</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="2"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
+      <c r="A36" s="2">
+        <v>35.0</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="2"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
+      <c r="A37" s="2">
+        <v>36.0</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="2"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
+      <c r="A38" s="2">
+        <v>37.0</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" s="2"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
+      <c r="A39" s="2">
+        <v>38.0</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="2"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
-      <c r="L40" s="5"/>
+      <c r="A40" s="2">
+        <v>39.0</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" s="2"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
+      <c r="A41" s="2">
+        <v>40.0</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" s="2"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
+      <c r="A42" s="2">
+        <v>41.0</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" s="2"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
+      <c r="A43" s="2">
+        <v>42.0</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" s="2"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
+      <c r="A44" s="2">
+        <v>43.0</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" s="2"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
+      <c r="A45" s="2">
+        <v>44.0</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" s="2"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
+      <c r="A46" s="2">
+        <v>45.0</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="47">
-      <c r="A47" s="2"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
+      <c r="A47" s="2">
+        <v>46.0</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="48">
-      <c r="A48" s="2"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
-      <c r="L48" s="5"/>
+      <c r="A48" s="2">
+        <v>47.0</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" s="2"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
+      <c r="A49" s="2">
+        <v>48.0</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" s="2"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="5"/>
-      <c r="L50" s="5"/>
+      <c r="A50" s="2">
+        <v>49.0</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D50" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" s="2"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
-      <c r="L51" s="5"/>
+      <c r="A51" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D51" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
-      <c r="L52" s="5"/>
+      <c r="A52" s="2">
+        <v>51.0</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="53">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
+      <c r="A53" s="2">
+        <v>52.0</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D53" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="54">
-      <c r="A54" s="5"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
-      <c r="L54" s="5"/>
+      <c r="A54" s="2">
+        <v>53.0</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D54" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="55">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
+      <c r="A55" s="2">
+        <v>54.0</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D55" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="56">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
-      <c r="J56" s="5"/>
-      <c r="K56" s="5"/>
-      <c r="L56" s="5"/>
+      <c r="A56" s="2">
+        <v>55.0</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D56" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="57">
-      <c r="A57" s="5"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
-      <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
-      <c r="J57" s="5"/>
-      <c r="K57" s="5"/>
-      <c r="L57" s="5"/>
+      <c r="A57" s="2">
+        <v>56.0</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D57" s="3">
+        <v>45909.0</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K57" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="58">
-      <c r="A58" s="5"/>
+      <c r="A58" s="2"/>
       <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
+      <c r="C58" s="2"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
-      <c r="J58" s="5"/>
-      <c r="K58" s="5"/>
-      <c r="L58" s="5"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
     </row>
     <row r="59">
-      <c r="A59" s="5"/>
+      <c r="A59" s="2"/>
       <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
+      <c r="C59" s="2"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
-      <c r="I59" s="5"/>
-      <c r="J59" s="5"/>
-      <c r="K59" s="5"/>
-      <c r="L59" s="5"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
     </row>
     <row r="60">
-      <c r="A60" s="5"/>
+      <c r="A60" s="2"/>
       <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
+      <c r="C60" s="2"/>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="5"/>
-      <c r="K60" s="5"/>
-      <c r="L60" s="5"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
     </row>
     <row r="61">
-      <c r="A61" s="5"/>
+      <c r="A61" s="2"/>
       <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
+      <c r="C61" s="2"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
-      <c r="I61" s="5"/>
-      <c r="J61" s="5"/>
-      <c r="K61" s="5"/>
-      <c r="L61" s="5"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
     </row>
     <row r="62">
-      <c r="A62" s="5"/>
+      <c r="A62" s="2"/>
       <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
+      <c r="C62" s="2"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
-      <c r="H62" s="5"/>
-      <c r="I62" s="5"/>
-      <c r="J62" s="5"/>
-      <c r="K62" s="5"/>
-      <c r="L62" s="5"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
     </row>
     <row r="63">
-      <c r="A63" s="5"/>
+      <c r="A63" s="2"/>
       <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
+      <c r="C63" s="2"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
-      <c r="K63" s="5"/>
-      <c r="L63" s="5"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
     </row>
     <row r="64">
-      <c r="A64" s="5"/>
+      <c r="A64" s="2"/>
       <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
+      <c r="C64" s="2"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
-      <c r="J64" s="5"/>
-      <c r="K64" s="5"/>
-      <c r="L64" s="5"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
     </row>
     <row r="65">
-      <c r="A65" s="5"/>
+      <c r="A65" s="2"/>
       <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
+      <c r="C65" s="2"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
-      <c r="J65" s="5"/>
-      <c r="K65" s="5"/>
-      <c r="L65" s="5"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
     </row>
     <row r="66">
-      <c r="A66" s="5"/>
+      <c r="A66" s="2"/>
       <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
+      <c r="C66" s="2"/>
       <c r="D66" s="5"/>
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
-      <c r="I66" s="5"/>
-      <c r="J66" s="5"/>
-      <c r="K66" s="5"/>
-      <c r="L66" s="5"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
     </row>
     <row r="67">
-      <c r="A67" s="5"/>
+      <c r="A67" s="2"/>
       <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
+      <c r="C67" s="2"/>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="5"/>
-      <c r="J67" s="5"/>
-      <c r="K67" s="5"/>
-      <c r="L67" s="5"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
     </row>
     <row r="68">
-      <c r="A68" s="5"/>
+      <c r="A68" s="2"/>
       <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
+      <c r="C68" s="2"/>
       <c r="D68" s="5"/>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="5"/>
-      <c r="J68" s="5"/>
-      <c r="K68" s="5"/>
-      <c r="L68" s="5"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
     </row>
     <row r="69">
-      <c r="A69" s="5"/>
+      <c r="A69" s="2"/>
       <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
+      <c r="C69" s="2"/>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2"/>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
     </row>
     <row r="70">
-      <c r="A70" s="5"/>
+      <c r="A70" s="2"/>
       <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
+      <c r="C70" s="2"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
-      <c r="H70" s="5"/>
-      <c r="I70" s="5"/>
-      <c r="J70" s="5"/>
-      <c r="K70" s="5"/>
-      <c r="L70" s="5"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
     </row>
     <row r="71">
-      <c r="A71" s="5"/>
+      <c r="A71" s="2"/>
       <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
+      <c r="C71" s="2"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
-      <c r="I71" s="5"/>
-      <c r="J71" s="5"/>
-      <c r="K71" s="5"/>
-      <c r="L71" s="5"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
     </row>
     <row r="72">
-      <c r="A72" s="5"/>
+      <c r="A72" s="2"/>
       <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
+      <c r="C72" s="2"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
-      <c r="H72" s="5"/>
-      <c r="I72" s="5"/>
-      <c r="J72" s="5"/>
-      <c r="K72" s="5"/>
-      <c r="L72" s="5"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="2"/>
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
     </row>
     <row r="73">
-      <c r="A73" s="5"/>
+      <c r="A73" s="2"/>
       <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
+      <c r="C73" s="2"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
       <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
-      <c r="J73" s="5"/>
-      <c r="K73" s="5"/>
-      <c r="L73" s="5"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
     </row>
     <row r="74">
-      <c r="A74" s="5"/>
+      <c r="A74" s="2"/>
       <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
+      <c r="C74" s="2"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-      <c r="L74" s="5"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
     </row>
     <row r="75">
-      <c r="A75" s="5"/>
+      <c r="A75" s="2"/>
       <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
+      <c r="C75" s="2"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
       <c r="G75" s="5"/>
-      <c r="H75" s="5"/>
-      <c r="I75" s="5"/>
-      <c r="J75" s="5"/>
-      <c r="K75" s="5"/>
-      <c r="L75" s="5"/>
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2"/>
+      <c r="K75" s="2"/>
+      <c r="L75" s="2"/>
     </row>
     <row r="76">
       <c r="A76" s="5"/>

</xml_diff>

<commit_message>
updated image based ad URLs to wotheat.com in ad index files
</commit_message>
<xml_diff>
--- a/google-ads/data/ad-index.xlsx
+++ b/google-ads/data/ad-index.xlsx
@@ -217,6 +217,9 @@
     <t>Join the fight — tanks, guns, and glory await!</t>
   </si>
   <si>
+    <t>https://www.wotheat.com</t>
+  </si>
+  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -425,9 +428,6 @@
   </si>
   <si>
     <t>⁦World of tanks: HEAT. Choose your Agent. Customize your loadout. Fight to win. Get ready to...⁩</t>
-  </si>
-  <si>
-    <t>https://www.wotheat.com</t>
   </si>
   <si>
     <t>CR17852167888085975041_2</t>
@@ -1631,17 +1631,17 @@
       <c r="G15" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>65</v>
@@ -1652,7 +1652,7 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>65</v>
@@ -1669,17 +1669,17 @@
       <c r="G16" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>65</v>
@@ -1690,7 +1690,7 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>65</v>
@@ -1702,22 +1702,22 @@
         <v>13</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H17" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>65</v>
@@ -1728,7 +1728,7 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>65</v>
@@ -1740,22 +1740,22 @@
         <v>13</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H18" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L18" s="5" t="s">
         <v>65</v>
@@ -1766,7 +1766,7 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>65</v>
@@ -1778,22 +1778,22 @@
         <v>13</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>65</v>
@@ -1804,7 +1804,7 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>65</v>
@@ -1816,22 +1816,22 @@
         <v>13</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L20" s="5" t="s">
         <v>65</v>
@@ -1842,7 +1842,7 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>65</v>
@@ -1854,22 +1854,22 @@
         <v>13</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>65</v>
@@ -1880,7 +1880,7 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>65</v>
@@ -1892,22 +1892,22 @@
         <v>13</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H22" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K22" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L22" s="5" t="s">
         <v>65</v>
@@ -1918,7 +1918,7 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>65</v>
@@ -1930,22 +1930,22 @@
         <v>13</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L23" s="5" t="s">
         <v>65</v>
@@ -1956,7 +1956,7 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>65</v>
@@ -1971,19 +1971,19 @@
         <v>17</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H24" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>65</v>
@@ -1994,7 +1994,7 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>65</v>
@@ -2011,17 +2011,17 @@
       <c r="G25" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>65</v>
@@ -2032,7 +2032,7 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>65</v>
@@ -2044,22 +2044,22 @@
         <v>13</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L26" s="5" t="s">
         <v>65</v>
@@ -2070,7 +2070,7 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>65</v>
@@ -2085,19 +2085,19 @@
         <v>17</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H27" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L27" s="5" t="s">
         <v>65</v>
@@ -2108,7 +2108,7 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>65</v>
@@ -2123,19 +2123,19 @@
         <v>17</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H28" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H28" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L28" s="5" t="s">
         <v>65</v>
@@ -2146,7 +2146,7 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>65</v>
@@ -2161,19 +2161,19 @@
         <v>17</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H29" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H29" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L29" s="5" t="s">
         <v>65</v>
@@ -2184,7 +2184,7 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>65</v>
@@ -2196,22 +2196,22 @@
         <v>13</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H30" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H30" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K30" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L30" s="5" t="s">
         <v>65</v>
@@ -2222,7 +2222,7 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>65</v>
@@ -2239,17 +2239,17 @@
       <c r="G31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K31" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L31" s="5" t="s">
         <v>65</v>
@@ -2260,7 +2260,7 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>65</v>
@@ -2275,19 +2275,19 @@
         <v>17</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H32" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H32" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K32" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L32" s="5" t="s">
         <v>65</v>
@@ -2298,7 +2298,7 @@
         <v>32.0</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>65</v>
@@ -2310,22 +2310,22 @@
         <v>13</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H33" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L33" s="5" t="s">
         <v>65</v>
@@ -2336,7 +2336,7 @@
         <v>33.0</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>65</v>
@@ -2348,22 +2348,22 @@
         <v>13</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L34" s="5" t="s">
         <v>65</v>
@@ -2374,7 +2374,7 @@
         <v>34.0</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>65</v>
@@ -2386,22 +2386,22 @@
         <v>13</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L35" s="5" t="s">
         <v>65</v>
@@ -2412,7 +2412,7 @@
         <v>35.0</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>65</v>
@@ -2429,17 +2429,17 @@
       <c r="G36" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="H36" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L36" s="5" t="s">
         <v>65</v>
@@ -2450,7 +2450,7 @@
         <v>36.0</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>65</v>
@@ -2467,17 +2467,17 @@
       <c r="G37" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="H37" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L37" s="5" t="s">
         <v>65</v>
@@ -2488,7 +2488,7 @@
         <v>37.0</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>65</v>
@@ -2500,22 +2500,22 @@
         <v>44</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="H38" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H38" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L38" s="5" t="s">
         <v>65</v>
@@ -2526,7 +2526,7 @@
         <v>38.0</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>65</v>
@@ -2541,19 +2541,19 @@
         <v>17</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H39" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H39" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L39" s="5" t="s">
         <v>65</v>
@@ -2564,7 +2564,7 @@
         <v>39.0</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>65</v>
@@ -2576,22 +2576,22 @@
         <v>44</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="H40" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L40" s="5" t="s">
         <v>65</v>
@@ -2602,7 +2602,7 @@
         <v>40.0</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>65</v>
@@ -2619,17 +2619,17 @@
       <c r="G41" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="H41" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L41" s="5" t="s">
         <v>65</v>
@@ -2640,7 +2640,7 @@
         <v>41.0</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>65</v>
@@ -2657,17 +2657,17 @@
       <c r="G42" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="H42" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L42" s="5" t="s">
         <v>65</v>
@@ -2678,7 +2678,7 @@
         <v>42.0</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>65</v>
@@ -2695,17 +2695,17 @@
       <c r="G43" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H43" s="3" t="s">
+      <c r="H43" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L43" s="5" t="s">
         <v>65</v>
@@ -2716,7 +2716,7 @@
         <v>43.0</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>65</v>
@@ -2728,22 +2728,22 @@
         <v>13</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="H44" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H44" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K44" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L44" s="5" t="s">
         <v>65</v>
@@ -2754,7 +2754,7 @@
         <v>44.0</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>65</v>
@@ -2766,22 +2766,22 @@
         <v>13</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H45" s="3" t="s">
+      <c r="H45" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>65</v>
@@ -2792,7 +2792,7 @@
         <v>45.0</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>65</v>
@@ -2804,22 +2804,22 @@
         <v>13</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="H46" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>65</v>
@@ -2830,7 +2830,7 @@
         <v>46.0</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>65</v>
@@ -2847,17 +2847,17 @@
       <c r="G47" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H47" s="3" t="s">
+      <c r="H47" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L47" s="5" t="s">
         <v>65</v>
@@ -2868,7 +2868,7 @@
         <v>47.0</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>65</v>
@@ -2885,17 +2885,17 @@
       <c r="G48" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H48" s="3" t="s">
+      <c r="H48" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K48" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L48" s="5" t="s">
         <v>65</v>
@@ -2906,7 +2906,7 @@
         <v>48.0</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>65</v>
@@ -2923,17 +2923,17 @@
       <c r="G49" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H49" s="3" t="s">
+      <c r="H49" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K49" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L49" s="5" t="s">
         <v>65</v>
@@ -2944,7 +2944,7 @@
         <v>49.0</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>65</v>
@@ -2956,22 +2956,22 @@
         <v>13</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H50" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H50" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I50" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K50" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L50" s="5" t="s">
         <v>65</v>
@@ -2982,7 +2982,7 @@
         <v>50.0</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>65</v>
@@ -2994,22 +2994,22 @@
         <v>13</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="H51" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H51" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K51" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L51" s="5" t="s">
         <v>65</v>
@@ -3020,7 +3020,7 @@
         <v>51.0</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>65</v>
@@ -3032,22 +3032,22 @@
         <v>13</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H52" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H52" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L52" s="5" t="s">
         <v>65</v>
@@ -3058,7 +3058,7 @@
         <v>52.0</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>65</v>
@@ -3075,17 +3075,17 @@
       <c r="G53" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H53" s="3" t="s">
+      <c r="H53" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K53" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L53" s="5" t="s">
         <v>65</v>
@@ -3096,7 +3096,7 @@
         <v>53.0</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>65</v>
@@ -3108,22 +3108,22 @@
         <v>44</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H54" s="3" t="s">
+      <c r="H54" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K54" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L54" s="5" t="s">
         <v>65</v>
@@ -3134,7 +3134,7 @@
         <v>54.0</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>65</v>
@@ -3151,17 +3151,17 @@
       <c r="G55" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H55" s="3" t="s">
+      <c r="H55" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K55" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L55" s="5" t="s">
         <v>65</v>
@@ -3172,7 +3172,7 @@
         <v>55.0</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>65</v>
@@ -3189,17 +3189,17 @@
       <c r="G56" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H56" s="3" t="s">
+      <c r="H56" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L56" s="5" t="s">
         <v>65</v>
@@ -3210,7 +3210,7 @@
         <v>56.0</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>65</v>
@@ -3222,22 +3222,22 @@
         <v>13</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H57" s="3" t="s">
+      <c r="H57" s="8" t="s">
         <v>68</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K57" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L57" s="5" t="s">
         <v>65</v>
@@ -3248,7 +3248,7 @@
         <v>57.0</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>65</v>
@@ -3260,22 +3260,22 @@
         <v>29</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L58" s="5" t="s">
         <v>65</v>
@@ -3286,7 +3286,7 @@
         <v>58.0</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>65</v>
@@ -3298,22 +3298,22 @@
         <v>13</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L59" s="5" t="s">
         <v>65</v>
@@ -3324,7 +3324,7 @@
         <v>59.0</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>65</v>
@@ -3336,22 +3336,22 @@
         <v>13</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I60" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L60" s="5" t="s">
         <v>65</v>
@@ -3380,16 +3380,16 @@
         <v>141</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I61" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L61" s="5" t="s">
         <v>65</v>
@@ -3418,16 +3418,16 @@
         <v>144</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I62" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K62" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L62" s="5" t="s">
         <v>65</v>
@@ -3450,22 +3450,22 @@
         <v>13</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>146</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I63" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K63" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L63" s="5" t="s">
         <v>65</v>
@@ -3494,16 +3494,16 @@
         <v>146</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I64" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K64" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L64" s="5" t="s">
         <v>65</v>
@@ -3532,16 +3532,16 @@
         <v>151</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I65" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K65" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L65" s="5" t="s">
         <v>65</v>
@@ -3570,16 +3570,16 @@
         <v>151</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I66" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K66" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L66" s="5" t="s">
         <v>65</v>
@@ -3608,16 +3608,16 @@
         <v>156</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I67" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K67" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L67" s="5" t="s">
         <v>65</v>
@@ -3646,16 +3646,16 @@
         <v>159</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I68" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K68" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L68" s="5" t="s">
         <v>65</v>
@@ -3684,16 +3684,16 @@
         <v>162</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I69" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K69" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L69" s="5" t="s">
         <v>65</v>
@@ -3722,16 +3722,16 @@
         <v>151</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I70" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K70" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L70" s="5" t="s">
         <v>65</v>
@@ -3760,16 +3760,16 @@
         <v>151</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K71" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L71" s="5" t="s">
         <v>65</v>
@@ -3798,16 +3798,16 @@
         <v>159</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I72" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K72" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L72" s="5" t="s">
         <v>65</v>
@@ -3836,16 +3836,16 @@
         <v>172</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I73" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K73" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L73" s="5" t="s">
         <v>65</v>
@@ -3874,16 +3874,16 @@
         <v>172</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I74" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K74" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L74" s="5" t="s">
         <v>65</v>
@@ -3912,16 +3912,16 @@
         <v>151</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I75" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K75" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L75" s="5" t="s">
         <v>65</v>
@@ -3950,16 +3950,16 @@
         <v>151</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I76" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K76" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L76" s="5" t="s">
         <v>65</v>
@@ -3988,16 +3988,16 @@
         <v>180</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I77" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K77" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L77" s="5" t="s">
         <v>65</v>
@@ -4026,16 +4026,16 @@
         <v>182</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I78" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K78" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L78" s="5" t="s">
         <v>65</v>
@@ -4064,16 +4064,16 @@
         <v>159</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I79" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K79" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L79" s="5" t="s">
         <v>65</v>
@@ -4102,16 +4102,16 @@
         <v>156</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I80" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K80" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L80" s="5" t="s">
         <v>65</v>
@@ -4140,16 +4140,16 @@
         <v>188</v>
       </c>
       <c r="H81" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I81" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K81" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L81" s="5" t="s">
         <v>65</v>
@@ -4178,16 +4178,16 @@
         <v>156</v>
       </c>
       <c r="H82" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I82" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K82" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L82" s="5" t="s">
         <v>65</v>
@@ -4216,16 +4216,16 @@
         <v>162</v>
       </c>
       <c r="H83" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I83" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K83" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L83" s="5" t="s">
         <v>65</v>
@@ -4254,16 +4254,16 @@
         <v>162</v>
       </c>
       <c r="H84" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I84" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K84" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L84" s="5" t="s">
         <v>65</v>
@@ -4292,16 +4292,16 @@
         <v>197</v>
       </c>
       <c r="H85" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I85" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K85" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L85" s="5" t="s">
         <v>65</v>
@@ -4330,16 +4330,16 @@
         <v>151</v>
       </c>
       <c r="H86" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I86" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K86" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L86" s="5" t="s">
         <v>65</v>
@@ -4368,16 +4368,16 @@
         <v>202</v>
       </c>
       <c r="H87" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I87" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K87" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L87" s="5" t="s">
         <v>65</v>
@@ -4406,16 +4406,16 @@
         <v>151</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I88" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K88" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L88" s="5" t="s">
         <v>65</v>
@@ -4444,16 +4444,16 @@
         <v>156</v>
       </c>
       <c r="H89" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I89" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K89" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L89" s="5" t="s">
         <v>65</v>
@@ -4482,16 +4482,16 @@
         <v>151</v>
       </c>
       <c r="H90" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I90" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K90" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L90" s="5" t="s">
         <v>65</v>
@@ -4520,16 +4520,16 @@
         <v>172</v>
       </c>
       <c r="H91" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I91" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L91" s="5" t="s">
         <v>65</v>
@@ -4558,16 +4558,16 @@
         <v>151</v>
       </c>
       <c r="H92" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I92" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L92" s="5" t="s">
         <v>65</v>
@@ -4596,16 +4596,16 @@
         <v>214</v>
       </c>
       <c r="H93" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I93" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K93" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L93" s="5" t="s">
         <v>65</v>
@@ -4634,16 +4634,16 @@
         <v>156</v>
       </c>
       <c r="H94" s="6" t="s">
-        <v>138</v>
+        <v>68</v>
       </c>
       <c r="I94" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K94" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L94" s="5" t="s">
         <v>65</v>
@@ -17372,44 +17372,87 @@
     <hyperlink r:id="rId24" ref="J13"/>
     <hyperlink r:id="rId25" ref="H14"/>
     <hyperlink r:id="rId26" ref="J14"/>
-    <hyperlink r:id="rId27" ref="H60"/>
-    <hyperlink r:id="rId28" ref="H61"/>
-    <hyperlink r:id="rId29" ref="H63"/>
-    <hyperlink r:id="rId30" ref="H64"/>
-    <hyperlink r:id="rId31" ref="H65"/>
-    <hyperlink r:id="rId32" ref="H66"/>
-    <hyperlink r:id="rId33" ref="H67"/>
-    <hyperlink r:id="rId34" ref="H68"/>
-    <hyperlink r:id="rId35" ref="H69"/>
-    <hyperlink r:id="rId36" ref="H70"/>
-    <hyperlink r:id="rId37" ref="H71"/>
-    <hyperlink r:id="rId38" ref="H72"/>
-    <hyperlink r:id="rId39" ref="H73"/>
-    <hyperlink r:id="rId40" ref="H74"/>
-    <hyperlink r:id="rId41" ref="H75"/>
-    <hyperlink r:id="rId42" ref="H76"/>
-    <hyperlink r:id="rId43" ref="H77"/>
-    <hyperlink r:id="rId44" ref="H78"/>
-    <hyperlink r:id="rId45" ref="H79"/>
-    <hyperlink r:id="rId46" ref="H80"/>
-    <hyperlink r:id="rId47" ref="H81"/>
-    <hyperlink r:id="rId48" ref="H82"/>
-    <hyperlink r:id="rId49" ref="H83"/>
-    <hyperlink r:id="rId50" ref="H84"/>
-    <hyperlink r:id="rId51" ref="H85"/>
-    <hyperlink r:id="rId52" ref="H86"/>
-    <hyperlink r:id="rId53" ref="H87"/>
-    <hyperlink r:id="rId54" ref="H88"/>
-    <hyperlink r:id="rId55" ref="H89"/>
-    <hyperlink r:id="rId56" ref="H90"/>
-    <hyperlink r:id="rId57" ref="H91"/>
-    <hyperlink r:id="rId58" ref="H92"/>
-    <hyperlink r:id="rId59" ref="H93"/>
-    <hyperlink r:id="rId60" ref="H94"/>
+    <hyperlink r:id="rId27" ref="H15"/>
+    <hyperlink r:id="rId28" ref="H16"/>
+    <hyperlink r:id="rId29" ref="H17"/>
+    <hyperlink r:id="rId30" ref="H18"/>
+    <hyperlink r:id="rId31" ref="H19"/>
+    <hyperlink r:id="rId32" ref="H20"/>
+    <hyperlink r:id="rId33" ref="H21"/>
+    <hyperlink r:id="rId34" ref="H22"/>
+    <hyperlink r:id="rId35" ref="H23"/>
+    <hyperlink r:id="rId36" ref="H24"/>
+    <hyperlink r:id="rId37" ref="H25"/>
+    <hyperlink r:id="rId38" ref="H26"/>
+    <hyperlink r:id="rId39" ref="H27"/>
+    <hyperlink r:id="rId40" ref="H28"/>
+    <hyperlink r:id="rId41" ref="H29"/>
+    <hyperlink r:id="rId42" ref="H30"/>
+    <hyperlink r:id="rId43" ref="H31"/>
+    <hyperlink r:id="rId44" ref="H32"/>
+    <hyperlink r:id="rId45" ref="H33"/>
+    <hyperlink r:id="rId46" ref="H34"/>
+    <hyperlink r:id="rId47" ref="H35"/>
+    <hyperlink r:id="rId48" ref="H36"/>
+    <hyperlink r:id="rId49" ref="H37"/>
+    <hyperlink r:id="rId50" ref="H38"/>
+    <hyperlink r:id="rId51" ref="H39"/>
+    <hyperlink r:id="rId52" ref="H40"/>
+    <hyperlink r:id="rId53" ref="H41"/>
+    <hyperlink r:id="rId54" ref="H42"/>
+    <hyperlink r:id="rId55" ref="H43"/>
+    <hyperlink r:id="rId56" ref="H44"/>
+    <hyperlink r:id="rId57" ref="H45"/>
+    <hyperlink r:id="rId58" ref="H46"/>
+    <hyperlink r:id="rId59" ref="H47"/>
+    <hyperlink r:id="rId60" ref="H48"/>
+    <hyperlink r:id="rId61" ref="H49"/>
+    <hyperlink r:id="rId62" ref="H50"/>
+    <hyperlink r:id="rId63" ref="H51"/>
+    <hyperlink r:id="rId64" ref="H52"/>
+    <hyperlink r:id="rId65" ref="H53"/>
+    <hyperlink r:id="rId66" ref="H54"/>
+    <hyperlink r:id="rId67" ref="H55"/>
+    <hyperlink r:id="rId68" ref="H56"/>
+    <hyperlink r:id="rId69" ref="H57"/>
+    <hyperlink r:id="rId70" ref="H60"/>
+    <hyperlink r:id="rId71" ref="H61"/>
+    <hyperlink r:id="rId72" ref="H63"/>
+    <hyperlink r:id="rId73" ref="H64"/>
+    <hyperlink r:id="rId74" ref="H65"/>
+    <hyperlink r:id="rId75" ref="H66"/>
+    <hyperlink r:id="rId76" ref="H67"/>
+    <hyperlink r:id="rId77" ref="H68"/>
+    <hyperlink r:id="rId78" ref="H69"/>
+    <hyperlink r:id="rId79" ref="H70"/>
+    <hyperlink r:id="rId80" ref="H71"/>
+    <hyperlink r:id="rId81" ref="H72"/>
+    <hyperlink r:id="rId82" ref="H73"/>
+    <hyperlink r:id="rId83" ref="H74"/>
+    <hyperlink r:id="rId84" ref="H75"/>
+    <hyperlink r:id="rId85" ref="H76"/>
+    <hyperlink r:id="rId86" ref="H77"/>
+    <hyperlink r:id="rId87" ref="H78"/>
+    <hyperlink r:id="rId88" ref="H79"/>
+    <hyperlink r:id="rId89" ref="H80"/>
+    <hyperlink r:id="rId90" ref="H81"/>
+    <hyperlink r:id="rId91" ref="H82"/>
+    <hyperlink r:id="rId92" ref="H83"/>
+    <hyperlink r:id="rId93" ref="H84"/>
+    <hyperlink r:id="rId94" ref="H85"/>
+    <hyperlink r:id="rId95" ref="H86"/>
+    <hyperlink r:id="rId96" ref="H87"/>
+    <hyperlink r:id="rId97" ref="H88"/>
+    <hyperlink r:id="rId98" ref="H89"/>
+    <hyperlink r:id="rId99" ref="H90"/>
+    <hyperlink r:id="rId100" ref="H91"/>
+    <hyperlink r:id="rId101" ref="H92"/>
+    <hyperlink r:id="rId102" ref="H93"/>
+    <hyperlink r:id="rId103" ref="H94"/>
   </hyperlinks>
-  <drawing r:id="rId61"/>
+  <drawing r:id="rId104"/>
   <tableParts count="1">
-    <tablePart r:id="rId63"/>
+    <tablePart r:id="rId106"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated ad URLs to wotheat.com without www
</commit_message>
<xml_diff>
--- a/google-ads/data/ad-index.xlsx
+++ b/google-ads/data/ad-index.xlsx
@@ -217,7 +217,7 @@
     <t>Join the fight — tanks, guns, and glory await!</t>
   </si>
   <si>
-    <t>https://www.wotheat.com</t>
+    <t>https://wotheat.com</t>
   </si>
   <si>
     <t>N/A</t>
@@ -406,7 +406,7 @@
     <t>⁦World of tanks: HEAT. Wybierz agenta. Dostosuj wyposażenie. Walcz, aby wygrać. Przygotuj się na nowy...⁩</t>
   </si>
   <si>
-    <t>https://www.wotheat.com/wishlist-now⁩</t>
+    <t>https://wotheat.com/wishlist-now⁩</t>
   </si>
   <si>
     <t>Text</t>

</xml_diff>